<commit_message>
Added a bunch of new data definitions, updated mimic item mapping. Added explorer option to 'investigate'. Added helper function to add mimic item mapping
</commit_message>
<xml_diff>
--- a/config/data_definitions.xlsx
+++ b/config/data_definitions.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18229"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\genkinjz\icu_ml_project\v5\config\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
@@ -17,12 +12,12 @@
     <sheet name="lists" sheetId="3" r:id="rId3"/>
     <sheet name="categories" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="137">
   <si>
     <t>component</t>
   </si>
@@ -162,6 +157,63 @@
     <t>phosphorous serum</t>
   </si>
   <si>
+    <t>prothrombin time</t>
+  </si>
+  <si>
+    <t>partial thromboplastin time</t>
+  </si>
+  <si>
+    <t>international normalized ratio</t>
+  </si>
+  <si>
+    <t>partial pressure of oxygen arterial</t>
+  </si>
+  <si>
+    <t>partial pressure of carbon dioxide arterial</t>
+  </si>
+  <si>
+    <t>oxygen saturation arterial</t>
+  </si>
+  <si>
+    <t>pH arterial</t>
+  </si>
+  <si>
+    <t>pH other</t>
+  </si>
+  <si>
+    <t>bicarbonate arterial</t>
+  </si>
+  <si>
+    <t>bicarbonate other</t>
+  </si>
+  <si>
+    <t>alanine aminotransferase serum</t>
+  </si>
+  <si>
+    <t>aspartate aminotransferase serum</t>
+  </si>
+  <si>
+    <t>alkaline phosphatase serum</t>
+  </si>
+  <si>
+    <t>fraction of inspired oxygen</t>
+  </si>
+  <si>
+    <t>positive end expiratory pressure</t>
+  </si>
+  <si>
+    <t>tidal volume</t>
+  </si>
+  <si>
+    <t>central venous pressure</t>
+  </si>
+  <si>
+    <t>central venous oxygen saturation</t>
+  </si>
+  <si>
+    <t>end tidal cardon dioxide</t>
+  </si>
+  <si>
     <t>beats/min</t>
   </si>
   <si>
@@ -231,6 +283,21 @@
     <t>umol/L</t>
   </si>
   <si>
+    <t>seconds</t>
+  </si>
+  <si>
+    <t>U/L</t>
+  </si>
+  <si>
+    <t>IU/L</t>
+  </si>
+  <si>
+    <t>cmH2O</t>
+  </si>
+  <si>
+    <t>mm/Hg</t>
+  </si>
+  <si>
     <t>qn</t>
   </si>
   <si>
@@ -277,6 +344,18 @@
   </si>
   <si>
     <t>basic metabolic panel</t>
+  </si>
+  <si>
+    <t>coagulation</t>
+  </si>
+  <si>
+    <t>arterial blood gas</t>
+  </si>
+  <si>
+    <t>liver function tests</t>
+  </si>
+  <si>
+    <t>ventilator settings</t>
   </si>
   <si>
     <t>table</t>
@@ -354,8 +433,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -418,14 +497,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -472,7 +543,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -504,27 +575,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -556,24 +609,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -749,19 +784,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H55"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H75"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A56" sqref="A56:XFD56"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="27.42578125" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -787,7 +817,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -795,13 +825,13 @@
         <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>46</v>
+        <v>65</v>
       </c>
       <c r="D2" t="s">
-        <v>69</v>
+        <v>93</v>
       </c>
       <c r="E2" t="s">
-        <v>71</v>
+        <v>95</v>
       </c>
       <c r="F2">
         <v>0</v>
@@ -810,7 +840,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -818,13 +848,13 @@
         <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>47</v>
+        <v>66</v>
       </c>
       <c r="D3" t="s">
-        <v>69</v>
+        <v>93</v>
       </c>
       <c r="E3" t="s">
-        <v>71</v>
+        <v>95</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -833,7 +863,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -841,13 +871,13 @@
         <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>47</v>
+        <v>66</v>
       </c>
       <c r="D4" t="s">
-        <v>69</v>
+        <v>93</v>
       </c>
       <c r="E4" t="s">
-        <v>71</v>
+        <v>95</v>
       </c>
       <c r="F4">
         <v>0</v>
@@ -856,7 +886,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -864,13 +894,13 @@
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>47</v>
+        <v>66</v>
       </c>
       <c r="D5" t="s">
-        <v>69</v>
+        <v>93</v>
       </c>
       <c r="E5" t="s">
-        <v>71</v>
+        <v>95</v>
       </c>
       <c r="F5">
         <v>0</v>
@@ -879,7 +909,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -887,13 +917,13 @@
         <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>48</v>
+        <v>67</v>
       </c>
       <c r="D6" t="s">
-        <v>69</v>
+        <v>93</v>
       </c>
       <c r="E6" t="s">
-        <v>71</v>
+        <v>95</v>
       </c>
       <c r="F6">
         <v>0</v>
@@ -902,7 +932,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -910,13 +940,13 @@
         <v>13</v>
       </c>
       <c r="C7" t="s">
-        <v>49</v>
+        <v>68</v>
       </c>
       <c r="D7" t="s">
-        <v>69</v>
+        <v>93</v>
       </c>
       <c r="E7" t="s">
-        <v>71</v>
+        <v>95</v>
       </c>
       <c r="F7">
         <v>0</v>
@@ -925,7 +955,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -933,13 +963,13 @@
         <v>14</v>
       </c>
       <c r="C8" t="s">
-        <v>50</v>
+        <v>69</v>
       </c>
       <c r="D8" t="s">
-        <v>69</v>
+        <v>93</v>
       </c>
       <c r="E8" t="s">
-        <v>71</v>
+        <v>95</v>
       </c>
       <c r="F8">
         <v>0</v>
@@ -948,7 +978,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -956,13 +986,13 @@
         <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>51</v>
+        <v>70</v>
       </c>
       <c r="D9" t="s">
-        <v>69</v>
+        <v>93</v>
       </c>
       <c r="E9" t="s">
-        <v>71</v>
+        <v>95</v>
       </c>
       <c r="F9">
         <v>0</v>
@@ -971,7 +1001,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -979,13 +1009,13 @@
         <v>16</v>
       </c>
       <c r="C10" t="s">
-        <v>52</v>
+        <v>71</v>
       </c>
       <c r="D10" t="s">
-        <v>69</v>
+        <v>93</v>
       </c>
       <c r="E10" t="s">
-        <v>71</v>
+        <v>95</v>
       </c>
       <c r="F10">
         <v>0</v>
@@ -994,7 +1024,7 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -1002,13 +1032,13 @@
         <v>16</v>
       </c>
       <c r="C11" t="s">
-        <v>53</v>
+        <v>72</v>
       </c>
       <c r="D11" t="s">
-        <v>69</v>
+        <v>93</v>
       </c>
       <c r="E11" t="s">
-        <v>71</v>
+        <v>95</v>
       </c>
       <c r="F11">
         <v>0</v>
@@ -1017,7 +1047,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -1025,13 +1055,13 @@
         <v>16</v>
       </c>
       <c r="C12" t="s">
-        <v>54</v>
+        <v>73</v>
       </c>
       <c r="D12" t="s">
-        <v>69</v>
+        <v>93</v>
       </c>
       <c r="E12" t="s">
-        <v>71</v>
+        <v>95</v>
       </c>
       <c r="F12">
         <v>0</v>
@@ -1040,7 +1070,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -1048,19 +1078,19 @@
         <v>17</v>
       </c>
       <c r="C13" t="s">
-        <v>55</v>
+        <v>74</v>
       </c>
       <c r="D13" t="s">
-        <v>70</v>
+        <v>94</v>
       </c>
       <c r="E13" t="s">
-        <v>71</v>
+        <v>95</v>
       </c>
       <c r="H13">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -1068,19 +1098,19 @@
         <v>18</v>
       </c>
       <c r="C14" t="s">
-        <v>55</v>
+        <v>74</v>
       </c>
       <c r="D14" t="s">
-        <v>70</v>
+        <v>94</v>
       </c>
       <c r="E14" t="s">
-        <v>71</v>
+        <v>95</v>
       </c>
       <c r="H14">
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -1088,19 +1118,19 @@
         <v>19</v>
       </c>
       <c r="C15" t="s">
-        <v>55</v>
+        <v>74</v>
       </c>
       <c r="D15" t="s">
-        <v>70</v>
+        <v>94</v>
       </c>
       <c r="E15" t="s">
-        <v>71</v>
+        <v>95</v>
       </c>
       <c r="H15">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -1108,13 +1138,13 @@
         <v>20</v>
       </c>
       <c r="C16" t="s">
-        <v>52</v>
+        <v>71</v>
       </c>
       <c r="D16" t="s">
-        <v>69</v>
+        <v>93</v>
       </c>
       <c r="E16" t="s">
-        <v>72</v>
+        <v>96</v>
       </c>
       <c r="F16">
         <v>0</v>
@@ -1123,7 +1153,7 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -1131,13 +1161,13 @@
         <v>20</v>
       </c>
       <c r="C17" t="s">
-        <v>53</v>
+        <v>72</v>
       </c>
       <c r="D17" t="s">
-        <v>69</v>
+        <v>93</v>
       </c>
       <c r="E17" t="s">
-        <v>72</v>
+        <v>96</v>
       </c>
       <c r="F17">
         <v>0</v>
@@ -1146,7 +1176,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -1154,13 +1184,13 @@
         <v>21</v>
       </c>
       <c r="C18" t="s">
-        <v>52</v>
+        <v>71</v>
       </c>
       <c r="D18" t="s">
-        <v>69</v>
+        <v>93</v>
       </c>
       <c r="E18" t="s">
-        <v>72</v>
+        <v>96</v>
       </c>
       <c r="F18">
         <v>0</v>
@@ -1169,7 +1199,7 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -1177,13 +1207,13 @@
         <v>21</v>
       </c>
       <c r="C19" t="s">
-        <v>53</v>
+        <v>72</v>
       </c>
       <c r="D19" t="s">
-        <v>69</v>
+        <v>93</v>
       </c>
       <c r="E19" t="s">
-        <v>72</v>
+        <v>96</v>
       </c>
       <c r="F19">
         <v>0</v>
@@ -1192,7 +1222,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -1200,13 +1230,13 @@
         <v>22</v>
       </c>
       <c r="C20" t="s">
-        <v>56</v>
+        <v>75</v>
       </c>
       <c r="D20" t="s">
-        <v>69</v>
+        <v>93</v>
       </c>
       <c r="E20" t="s">
-        <v>72</v>
+        <v>96</v>
       </c>
       <c r="F20">
         <v>0</v>
@@ -1215,7 +1245,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -1223,13 +1253,13 @@
         <v>22</v>
       </c>
       <c r="C21" t="s">
-        <v>57</v>
+        <v>76</v>
       </c>
       <c r="D21" t="s">
-        <v>69</v>
+        <v>93</v>
       </c>
       <c r="E21" t="s">
-        <v>72</v>
+        <v>96</v>
       </c>
       <c r="F21">
         <v>0</v>
@@ -1238,7 +1268,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -1246,13 +1276,13 @@
         <v>22</v>
       </c>
       <c r="C22" t="s">
-        <v>58</v>
+        <v>77</v>
       </c>
       <c r="D22" t="s">
-        <v>69</v>
+        <v>93</v>
       </c>
       <c r="E22" t="s">
-        <v>72</v>
+        <v>96</v>
       </c>
       <c r="F22">
         <v>0</v>
@@ -1261,7 +1291,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -1272,10 +1302,10 @@
         <v>1</v>
       </c>
       <c r="D23" t="s">
-        <v>69</v>
+        <v>93</v>
       </c>
       <c r="E23" t="s">
-        <v>72</v>
+        <v>96</v>
       </c>
       <c r="F23">
         <v>0</v>
@@ -1284,7 +1314,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -1292,13 +1322,13 @@
         <v>23</v>
       </c>
       <c r="C24" t="s">
-        <v>59</v>
+        <v>78</v>
       </c>
       <c r="D24" t="s">
-        <v>69</v>
+        <v>93</v>
       </c>
       <c r="E24" t="s">
-        <v>72</v>
+        <v>96</v>
       </c>
       <c r="F24">
         <v>0</v>
@@ -1307,7 +1337,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -1315,13 +1345,13 @@
         <v>24</v>
       </c>
       <c r="C25" t="s">
-        <v>60</v>
+        <v>79</v>
       </c>
       <c r="D25" t="s">
-        <v>69</v>
+        <v>93</v>
       </c>
       <c r="E25" t="s">
-        <v>71</v>
+        <v>95</v>
       </c>
       <c r="F25">
         <v>0</v>
@@ -1330,7 +1360,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -1338,13 +1368,13 @@
         <v>24</v>
       </c>
       <c r="C26" t="s">
-        <v>61</v>
+        <v>80</v>
       </c>
       <c r="D26" t="s">
-        <v>69</v>
+        <v>93</v>
       </c>
       <c r="E26" t="s">
-        <v>71</v>
+        <v>95</v>
       </c>
       <c r="F26">
         <v>0</v>
@@ -1353,7 +1383,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -1361,13 +1391,13 @@
         <v>25</v>
       </c>
       <c r="C27" t="s">
-        <v>62</v>
+        <v>81</v>
       </c>
       <c r="D27" t="s">
-        <v>69</v>
+        <v>93</v>
       </c>
       <c r="E27" t="s">
-        <v>71</v>
+        <v>95</v>
       </c>
       <c r="F27">
         <v>0</v>
@@ -1376,7 +1406,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -1384,13 +1414,13 @@
         <v>26</v>
       </c>
       <c r="C28" t="s">
-        <v>63</v>
+        <v>82</v>
       </c>
       <c r="D28" t="s">
-        <v>69</v>
+        <v>93</v>
       </c>
       <c r="E28" t="s">
-        <v>71</v>
+        <v>95</v>
       </c>
       <c r="F28">
         <v>0</v>
@@ -1399,7 +1429,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -1407,13 +1437,13 @@
         <v>27</v>
       </c>
       <c r="C29" t="s">
-        <v>64</v>
+        <v>83</v>
       </c>
       <c r="D29" t="s">
-        <v>69</v>
+        <v>93</v>
       </c>
       <c r="E29" t="s">
-        <v>71</v>
+        <v>95</v>
       </c>
       <c r="F29">
         <v>0</v>
@@ -1422,7 +1452,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -1430,13 +1460,13 @@
         <v>28</v>
       </c>
       <c r="C30" t="s">
-        <v>50</v>
+        <v>69</v>
       </c>
       <c r="D30" t="s">
-        <v>69</v>
+        <v>93</v>
       </c>
       <c r="E30" t="s">
-        <v>71</v>
+        <v>95</v>
       </c>
       <c r="F30">
         <v>0</v>
@@ -1445,7 +1475,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -1453,13 +1483,13 @@
         <v>29</v>
       </c>
       <c r="C31" t="s">
-        <v>65</v>
+        <v>84</v>
       </c>
       <c r="D31" t="s">
-        <v>69</v>
+        <v>93</v>
       </c>
       <c r="E31" t="s">
-        <v>71</v>
+        <v>95</v>
       </c>
       <c r="F31">
         <v>0</v>
@@ -1468,7 +1498,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -1476,13 +1506,13 @@
         <v>30</v>
       </c>
       <c r="C32" t="s">
-        <v>66</v>
+        <v>85</v>
       </c>
       <c r="D32" t="s">
-        <v>69</v>
+        <v>93</v>
       </c>
       <c r="E32" t="s">
-        <v>71</v>
+        <v>95</v>
       </c>
       <c r="F32">
         <v>0</v>
@@ -1491,7 +1521,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -1499,13 +1529,13 @@
         <v>31</v>
       </c>
       <c r="C33" t="s">
-        <v>62</v>
+        <v>81</v>
       </c>
       <c r="D33" t="s">
-        <v>69</v>
+        <v>93</v>
       </c>
       <c r="E33" t="s">
-        <v>71</v>
+        <v>95</v>
       </c>
       <c r="F33">
         <v>0</v>
@@ -1514,7 +1544,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -1522,13 +1552,13 @@
         <v>32</v>
       </c>
       <c r="C34" t="s">
-        <v>50</v>
+        <v>69</v>
       </c>
       <c r="D34" t="s">
-        <v>69</v>
+        <v>93</v>
       </c>
       <c r="E34" t="s">
-        <v>71</v>
+        <v>95</v>
       </c>
       <c r="F34">
         <v>0</v>
@@ -1537,7 +1567,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -1545,13 +1575,13 @@
         <v>33</v>
       </c>
       <c r="C35" t="s">
-        <v>63</v>
+        <v>82</v>
       </c>
       <c r="D35" t="s">
-        <v>69</v>
+        <v>93</v>
       </c>
       <c r="E35" t="s">
-        <v>71</v>
+        <v>95</v>
       </c>
       <c r="F35">
         <v>0</v>
@@ -1560,7 +1590,7 @@
         <v>5000000</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7">
       <c r="A36" s="1">
         <v>34</v>
       </c>
@@ -1568,13 +1598,13 @@
         <v>34</v>
       </c>
       <c r="C36" t="s">
-        <v>67</v>
+        <v>86</v>
       </c>
       <c r="D36" t="s">
-        <v>69</v>
+        <v>93</v>
       </c>
       <c r="E36" t="s">
-        <v>71</v>
+        <v>95</v>
       </c>
       <c r="F36">
         <v>0</v>
@@ -1583,7 +1613,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7">
       <c r="A37" s="1">
         <v>35</v>
       </c>
@@ -1591,13 +1621,13 @@
         <v>34</v>
       </c>
       <c r="C37" t="s">
-        <v>60</v>
+        <v>79</v>
       </c>
       <c r="D37" t="s">
-        <v>69</v>
+        <v>93</v>
       </c>
       <c r="E37" t="s">
-        <v>71</v>
+        <v>95</v>
       </c>
       <c r="F37">
         <v>0</v>
@@ -1606,7 +1636,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7">
       <c r="A38" s="1">
         <v>36</v>
       </c>
@@ -1614,13 +1644,13 @@
         <v>35</v>
       </c>
       <c r="C38" t="s">
-        <v>67</v>
+        <v>86</v>
       </c>
       <c r="D38" t="s">
-        <v>69</v>
+        <v>93</v>
       </c>
       <c r="E38" t="s">
-        <v>71</v>
+        <v>95</v>
       </c>
       <c r="F38">
         <v>0</v>
@@ -1629,7 +1659,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7">
       <c r="A39" s="1">
         <v>37</v>
       </c>
@@ -1637,13 +1667,13 @@
         <v>35</v>
       </c>
       <c r="C39" t="s">
-        <v>60</v>
+        <v>79</v>
       </c>
       <c r="D39" t="s">
-        <v>69</v>
+        <v>93</v>
       </c>
       <c r="E39" t="s">
-        <v>71</v>
+        <v>95</v>
       </c>
       <c r="F39">
         <v>0</v>
@@ -1652,7 +1682,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7">
       <c r="A40" s="1">
         <v>38</v>
       </c>
@@ -1660,13 +1690,13 @@
         <v>36</v>
       </c>
       <c r="C40" t="s">
-        <v>60</v>
+        <v>79</v>
       </c>
       <c r="D40" t="s">
-        <v>69</v>
+        <v>93</v>
       </c>
       <c r="E40" t="s">
-        <v>71</v>
+        <v>95</v>
       </c>
       <c r="F40">
         <v>0</v>
@@ -1675,7 +1705,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7">
       <c r="A41" s="1">
         <v>39</v>
       </c>
@@ -1683,13 +1713,13 @@
         <v>37</v>
       </c>
       <c r="C41" t="s">
-        <v>60</v>
+        <v>79</v>
       </c>
       <c r="D41" t="s">
-        <v>69</v>
+        <v>93</v>
       </c>
       <c r="E41" t="s">
-        <v>71</v>
+        <v>95</v>
       </c>
       <c r="F41">
         <v>0</v>
@@ -1698,7 +1728,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7">
       <c r="A42" s="1">
         <v>40</v>
       </c>
@@ -1706,13 +1736,13 @@
         <v>38</v>
       </c>
       <c r="C42" t="s">
-        <v>60</v>
+        <v>79</v>
       </c>
       <c r="D42" t="s">
-        <v>69</v>
+        <v>93</v>
       </c>
       <c r="E42" t="s">
-        <v>71</v>
+        <v>95</v>
       </c>
       <c r="F42">
         <v>0</v>
@@ -1721,7 +1751,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7">
       <c r="A43" s="1">
         <v>41</v>
       </c>
@@ -1729,13 +1759,13 @@
         <v>38</v>
       </c>
       <c r="C43" t="s">
-        <v>61</v>
+        <v>80</v>
       </c>
       <c r="D43" t="s">
-        <v>69</v>
+        <v>93</v>
       </c>
       <c r="E43" t="s">
-        <v>71</v>
+        <v>95</v>
       </c>
       <c r="F43">
         <v>0</v>
@@ -1744,7 +1774,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7">
       <c r="A44" s="1">
         <v>42</v>
       </c>
@@ -1752,13 +1782,13 @@
         <v>39</v>
       </c>
       <c r="C44" t="s">
-        <v>68</v>
+        <v>87</v>
       </c>
       <c r="D44" t="s">
-        <v>69</v>
+        <v>93</v>
       </c>
       <c r="E44" t="s">
-        <v>71</v>
+        <v>95</v>
       </c>
       <c r="F44">
         <v>0</v>
@@ -1767,7 +1797,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7">
       <c r="A45" s="1">
         <v>43</v>
       </c>
@@ -1775,13 +1805,13 @@
         <v>39</v>
       </c>
       <c r="C45" t="s">
-        <v>61</v>
+        <v>80</v>
       </c>
       <c r="D45" t="s">
-        <v>69</v>
+        <v>93</v>
       </c>
       <c r="E45" t="s">
-        <v>71</v>
+        <v>95</v>
       </c>
       <c r="F45">
         <v>0</v>
@@ -1790,7 +1820,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7">
       <c r="A46" s="1">
         <v>44</v>
       </c>
@@ -1798,13 +1828,13 @@
         <v>40</v>
       </c>
       <c r="C46" t="s">
-        <v>60</v>
+        <v>79</v>
       </c>
       <c r="D46" t="s">
-        <v>69</v>
+        <v>93</v>
       </c>
       <c r="E46" t="s">
-        <v>71</v>
+        <v>95</v>
       </c>
       <c r="F46">
         <v>0</v>
@@ -1813,7 +1843,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7">
       <c r="A47" s="1">
         <v>45</v>
       </c>
@@ -1821,13 +1851,13 @@
         <v>40</v>
       </c>
       <c r="C47" t="s">
-        <v>61</v>
+        <v>80</v>
       </c>
       <c r="D47" t="s">
-        <v>69</v>
+        <v>93</v>
       </c>
       <c r="E47" t="s">
-        <v>71</v>
+        <v>95</v>
       </c>
       <c r="F47">
         <v>0</v>
@@ -1836,7 +1866,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7">
       <c r="A48" s="1">
         <v>46</v>
       </c>
@@ -1844,13 +1874,13 @@
         <v>41</v>
       </c>
       <c r="C48" t="s">
-        <v>60</v>
+        <v>79</v>
       </c>
       <c r="D48" t="s">
-        <v>69</v>
+        <v>93</v>
       </c>
       <c r="E48" t="s">
-        <v>71</v>
+        <v>95</v>
       </c>
       <c r="F48">
         <v>0</v>
@@ -1859,7 +1889,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7">
       <c r="A49" s="1">
         <v>47</v>
       </c>
@@ -1867,13 +1897,13 @@
         <v>41</v>
       </c>
       <c r="C49" t="s">
-        <v>61</v>
+        <v>80</v>
       </c>
       <c r="D49" t="s">
-        <v>69</v>
+        <v>93</v>
       </c>
       <c r="E49" t="s">
-        <v>71</v>
+        <v>95</v>
       </c>
       <c r="F49">
         <v>0</v>
@@ -1882,7 +1912,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7">
       <c r="A50" s="1">
         <v>48</v>
       </c>
@@ -1890,13 +1920,13 @@
         <v>42</v>
       </c>
       <c r="C50" t="s">
-        <v>60</v>
+        <v>79</v>
       </c>
       <c r="D50" t="s">
-        <v>69</v>
+        <v>93</v>
       </c>
       <c r="E50" t="s">
-        <v>71</v>
+        <v>95</v>
       </c>
       <c r="F50">
         <v>0</v>
@@ -1905,7 +1935,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7">
       <c r="A51" s="1">
         <v>49</v>
       </c>
@@ -1913,13 +1943,13 @@
         <v>42</v>
       </c>
       <c r="C51" t="s">
-        <v>61</v>
+        <v>80</v>
       </c>
       <c r="D51" t="s">
-        <v>69</v>
+        <v>93</v>
       </c>
       <c r="E51" t="s">
-        <v>71</v>
+        <v>95</v>
       </c>
       <c r="F51">
         <v>0</v>
@@ -1928,7 +1958,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7">
       <c r="A52" s="1">
         <v>50</v>
       </c>
@@ -1936,13 +1966,13 @@
         <v>43</v>
       </c>
       <c r="C52" t="s">
-        <v>60</v>
+        <v>79</v>
       </c>
       <c r="D52" t="s">
-        <v>69</v>
+        <v>93</v>
       </c>
       <c r="E52" t="s">
-        <v>71</v>
+        <v>95</v>
       </c>
       <c r="F52">
         <v>0</v>
@@ -1951,7 +1981,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7">
       <c r="A53" s="1">
         <v>51</v>
       </c>
@@ -1959,13 +1989,13 @@
         <v>43</v>
       </c>
       <c r="C53" t="s">
-        <v>61</v>
+        <v>80</v>
       </c>
       <c r="D53" t="s">
-        <v>69</v>
+        <v>93</v>
       </c>
       <c r="E53" t="s">
-        <v>71</v>
+        <v>95</v>
       </c>
       <c r="F53">
         <v>0</v>
@@ -1974,7 +2004,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7">
       <c r="A54" s="1">
         <v>52</v>
       </c>
@@ -1982,13 +2012,13 @@
         <v>44</v>
       </c>
       <c r="C54" t="s">
-        <v>61</v>
+        <v>80</v>
       </c>
       <c r="D54" t="s">
-        <v>69</v>
+        <v>93</v>
       </c>
       <c r="E54" t="s">
-        <v>71</v>
+        <v>95</v>
       </c>
       <c r="F54">
         <v>0</v>
@@ -1997,7 +2027,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7">
       <c r="A55" s="1">
         <v>53</v>
       </c>
@@ -2005,19 +2035,479 @@
         <v>45</v>
       </c>
       <c r="C55" t="s">
-        <v>61</v>
+        <v>80</v>
       </c>
       <c r="D55" t="s">
-        <v>69</v>
+        <v>93</v>
       </c>
       <c r="E55" t="s">
-        <v>71</v>
+        <v>95</v>
       </c>
       <c r="F55">
         <v>0</v>
       </c>
       <c r="G55">
         <v>100</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7">
+      <c r="A56" s="1">
+        <v>54</v>
+      </c>
+      <c r="B56" t="s">
+        <v>46</v>
+      </c>
+      <c r="C56" t="s">
+        <v>88</v>
+      </c>
+      <c r="D56" t="s">
+        <v>93</v>
+      </c>
+      <c r="E56" t="s">
+        <v>95</v>
+      </c>
+      <c r="F56">
+        <v>0</v>
+      </c>
+      <c r="G56">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7">
+      <c r="A57" s="1">
+        <v>55</v>
+      </c>
+      <c r="B57" t="s">
+        <v>47</v>
+      </c>
+      <c r="C57" t="s">
+        <v>88</v>
+      </c>
+      <c r="D57" t="s">
+        <v>93</v>
+      </c>
+      <c r="E57" t="s">
+        <v>95</v>
+      </c>
+      <c r="F57">
+        <v>0</v>
+      </c>
+      <c r="G57">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7">
+      <c r="A58" s="1">
+        <v>56</v>
+      </c>
+      <c r="B58" t="s">
+        <v>48</v>
+      </c>
+      <c r="C58" t="s">
+        <v>74</v>
+      </c>
+      <c r="D58" t="s">
+        <v>93</v>
+      </c>
+      <c r="E58" t="s">
+        <v>95</v>
+      </c>
+      <c r="F58">
+        <v>0</v>
+      </c>
+      <c r="G58">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7">
+      <c r="A59" s="1">
+        <v>57</v>
+      </c>
+      <c r="B59" t="s">
+        <v>49</v>
+      </c>
+      <c r="C59" t="s">
+        <v>66</v>
+      </c>
+      <c r="D59" t="s">
+        <v>93</v>
+      </c>
+      <c r="E59" t="s">
+        <v>95</v>
+      </c>
+      <c r="F59">
+        <v>0</v>
+      </c>
+      <c r="G59">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7">
+      <c r="A60" s="1">
+        <v>58</v>
+      </c>
+      <c r="B60" t="s">
+        <v>50</v>
+      </c>
+      <c r="C60" t="s">
+        <v>66</v>
+      </c>
+      <c r="D60" t="s">
+        <v>93</v>
+      </c>
+      <c r="E60" t="s">
+        <v>95</v>
+      </c>
+      <c r="F60">
+        <v>0</v>
+      </c>
+      <c r="G60">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7">
+      <c r="A61" s="1">
+        <v>59</v>
+      </c>
+      <c r="B61" t="s">
+        <v>51</v>
+      </c>
+      <c r="C61" t="s">
+        <v>69</v>
+      </c>
+      <c r="D61" t="s">
+        <v>93</v>
+      </c>
+      <c r="E61" t="s">
+        <v>95</v>
+      </c>
+      <c r="F61">
+        <v>0</v>
+      </c>
+      <c r="G61">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7">
+      <c r="A62" s="1">
+        <v>60</v>
+      </c>
+      <c r="B62" t="s">
+        <v>52</v>
+      </c>
+      <c r="C62" t="s">
+        <v>74</v>
+      </c>
+      <c r="D62" t="s">
+        <v>93</v>
+      </c>
+      <c r="E62" t="s">
+        <v>95</v>
+      </c>
+      <c r="F62">
+        <v>0</v>
+      </c>
+      <c r="G62">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7">
+      <c r="A63" s="1">
+        <v>61</v>
+      </c>
+      <c r="B63" t="s">
+        <v>53</v>
+      </c>
+      <c r="C63" t="s">
+        <v>74</v>
+      </c>
+      <c r="D63" t="s">
+        <v>93</v>
+      </c>
+      <c r="E63" t="s">
+        <v>95</v>
+      </c>
+      <c r="F63">
+        <v>0</v>
+      </c>
+      <c r="G63">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7">
+      <c r="A64" s="1">
+        <v>62</v>
+      </c>
+      <c r="B64" t="s">
+        <v>54</v>
+      </c>
+      <c r="C64" t="s">
+        <v>86</v>
+      </c>
+      <c r="D64" t="s">
+        <v>93</v>
+      </c>
+      <c r="E64" t="s">
+        <v>95</v>
+      </c>
+      <c r="F64">
+        <v>0</v>
+      </c>
+      <c r="G64">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7">
+      <c r="A65" s="1">
+        <v>63</v>
+      </c>
+      <c r="B65" t="s">
+        <v>55</v>
+      </c>
+      <c r="C65" t="s">
+        <v>86</v>
+      </c>
+      <c r="D65" t="s">
+        <v>93</v>
+      </c>
+      <c r="E65" t="s">
+        <v>95</v>
+      </c>
+      <c r="F65">
+        <v>0</v>
+      </c>
+      <c r="G65">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7">
+      <c r="A66" s="1">
+        <v>64</v>
+      </c>
+      <c r="B66" t="s">
+        <v>56</v>
+      </c>
+      <c r="C66" t="s">
+        <v>89</v>
+      </c>
+      <c r="D66" t="s">
+        <v>93</v>
+      </c>
+      <c r="E66" t="s">
+        <v>95</v>
+      </c>
+      <c r="F66">
+        <v>0</v>
+      </c>
+      <c r="G66">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7">
+      <c r="A67" s="1">
+        <v>65</v>
+      </c>
+      <c r="B67" t="s">
+        <v>57</v>
+      </c>
+      <c r="C67" t="s">
+        <v>89</v>
+      </c>
+      <c r="D67" t="s">
+        <v>93</v>
+      </c>
+      <c r="E67" t="s">
+        <v>95</v>
+      </c>
+      <c r="F67">
+        <v>0</v>
+      </c>
+      <c r="G67">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7">
+      <c r="A68" s="1">
+        <v>66</v>
+      </c>
+      <c r="B68" t="s">
+        <v>58</v>
+      </c>
+      <c r="C68" t="s">
+        <v>90</v>
+      </c>
+      <c r="D68" t="s">
+        <v>93</v>
+      </c>
+      <c r="E68" t="s">
+        <v>95</v>
+      </c>
+      <c r="F68">
+        <v>0</v>
+      </c>
+      <c r="G68">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7">
+      <c r="A69" s="1">
+        <v>67</v>
+      </c>
+      <c r="B69" t="s">
+        <v>59</v>
+      </c>
+      <c r="C69" t="s">
+        <v>69</v>
+      </c>
+      <c r="D69" t="s">
+        <v>93</v>
+      </c>
+      <c r="E69" t="s">
+        <v>95</v>
+      </c>
+      <c r="F69">
+        <v>0</v>
+      </c>
+      <c r="G69">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7">
+      <c r="A70" s="1">
+        <v>68</v>
+      </c>
+      <c r="B70" t="s">
+        <v>59</v>
+      </c>
+      <c r="C70" t="s">
+        <v>74</v>
+      </c>
+      <c r="D70" t="s">
+        <v>93</v>
+      </c>
+      <c r="E70" t="s">
+        <v>95</v>
+      </c>
+      <c r="F70">
+        <v>0</v>
+      </c>
+      <c r="G70">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7">
+      <c r="A71" s="1">
+        <v>69</v>
+      </c>
+      <c r="B71" t="s">
+        <v>60</v>
+      </c>
+      <c r="C71" t="s">
+        <v>91</v>
+      </c>
+      <c r="D71" t="s">
+        <v>93</v>
+      </c>
+      <c r="E71" t="s">
+        <v>95</v>
+      </c>
+      <c r="F71">
+        <v>0</v>
+      </c>
+      <c r="G71">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7">
+      <c r="A72" s="1">
+        <v>70</v>
+      </c>
+      <c r="B72" t="s">
+        <v>61</v>
+      </c>
+      <c r="C72" t="s">
+        <v>71</v>
+      </c>
+      <c r="D72" t="s">
+        <v>93</v>
+      </c>
+      <c r="E72" t="s">
+        <v>95</v>
+      </c>
+      <c r="F72">
+        <v>0</v>
+      </c>
+      <c r="G72">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7">
+      <c r="A73" s="1">
+        <v>71</v>
+      </c>
+      <c r="B73" t="s">
+        <v>62</v>
+      </c>
+      <c r="C73" t="s">
+        <v>92</v>
+      </c>
+      <c r="D73" t="s">
+        <v>93</v>
+      </c>
+      <c r="E73" t="s">
+        <v>95</v>
+      </c>
+      <c r="F73">
+        <v>0</v>
+      </c>
+      <c r="G73">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7">
+      <c r="A74" s="1">
+        <v>72</v>
+      </c>
+      <c r="B74" t="s">
+        <v>63</v>
+      </c>
+      <c r="C74" t="s">
+        <v>69</v>
+      </c>
+      <c r="D74" t="s">
+        <v>93</v>
+      </c>
+      <c r="E74" t="s">
+        <v>95</v>
+      </c>
+      <c r="F74">
+        <v>0</v>
+      </c>
+      <c r="G74">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7">
+      <c r="A75" s="1">
+        <v>73</v>
+      </c>
+      <c r="B75" t="s">
+        <v>64</v>
+      </c>
+      <c r="C75" t="s">
+        <v>66</v>
+      </c>
+      <c r="D75" t="s">
+        <v>93</v>
+      </c>
+      <c r="E75" t="s">
+        <v>95</v>
+      </c>
+      <c r="F75">
+        <v>0</v>
+      </c>
+      <c r="G75">
+        <v>1000</v>
       </c>
     </row>
   </sheetData>
@@ -2026,69 +2516,69 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>74</v>
+        <v>98</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>73</v>
+        <v>97</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>75</v>
+        <v>99</v>
       </c>
       <c r="C2">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>76</v>
+        <v>100</v>
       </c>
       <c r="C3">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>77</v>
+        <v>101</v>
       </c>
       <c r="C4">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>78</v>
+        <v>102</v>
       </c>
       <c r="C5">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -2099,7 +2589,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -2110,18 +2600,18 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3">
       <c r="A8" s="1">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>79</v>
+        <v>103</v>
       </c>
       <c r="C8">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -2132,7 +2622,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -2143,18 +2633,18 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3">
       <c r="A11" s="1">
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>80</v>
+        <v>104</v>
       </c>
       <c r="C11">
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -2165,48 +2655,103 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3">
       <c r="A13" s="1">
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>81</v>
+        <v>105</v>
       </c>
       <c r="C13">
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3">
       <c r="A14" s="1">
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>82</v>
+        <v>106</v>
       </c>
       <c r="C14">
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3">
       <c r="A15" s="1">
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>83</v>
+        <v>107</v>
       </c>
       <c r="C15">
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3">
       <c r="A16" s="1">
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>84</v>
+        <v>108</v>
       </c>
       <c r="C16">
         <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="1">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>109</v>
+      </c>
+      <c r="C17">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="1">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>110</v>
+      </c>
+      <c r="C18">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="1">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>110</v>
+      </c>
+      <c r="C19">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="1">
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
+        <v>111</v>
+      </c>
+      <c r="C20">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="1">
+        <v>19</v>
+      </c>
+      <c r="B21" t="s">
+        <v>112</v>
+      </c>
+      <c r="C21">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -2215,33 +2760,33 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D75"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D92"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>85</v>
+        <v>113</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>86</v>
+        <v>114</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>88</v>
+        <v>116</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -2250,12 +2795,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" s="1">
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>88</v>
+        <v>116</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -2264,12 +2809,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" s="1">
         <v>0</v>
       </c>
       <c r="B4" t="s">
-        <v>88</v>
+        <v>116</v>
       </c>
       <c r="C4">
         <v>2</v>
@@ -2278,12 +2823,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="A5" s="1">
         <v>0</v>
       </c>
       <c r="B5" t="s">
-        <v>88</v>
+        <v>116</v>
       </c>
       <c r="C5">
         <v>3</v>
@@ -2292,12 +2837,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="A6" s="1">
         <v>0</v>
       </c>
       <c r="B6" t="s">
-        <v>88</v>
+        <v>116</v>
       </c>
       <c r="C6">
         <v>4</v>
@@ -2306,12 +2851,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" s="1">
         <v>0</v>
       </c>
       <c r="B7" t="s">
-        <v>88</v>
+        <v>116</v>
       </c>
       <c r="C7">
         <v>5</v>
@@ -2320,12 +2865,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" s="1">
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>88</v>
+        <v>116</v>
       </c>
       <c r="C8">
         <v>10</v>
@@ -2334,12 +2879,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" s="1">
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>88</v>
+        <v>116</v>
       </c>
       <c r="C9">
         <v>11</v>
@@ -2348,12 +2893,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" s="1">
         <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>88</v>
+        <v>116</v>
       </c>
       <c r="C10">
         <v>12</v>
@@ -2362,12 +2907,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4">
       <c r="A11" s="1">
         <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>88</v>
+        <v>116</v>
       </c>
       <c r="C11">
         <v>13</v>
@@ -2376,12 +2921,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="A12" s="1">
         <v>1</v>
       </c>
       <c r="B12" t="s">
-        <v>88</v>
+        <v>116</v>
       </c>
       <c r="C12">
         <v>14</v>
@@ -2390,12 +2935,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="A13" s="1">
         <v>2</v>
       </c>
       <c r="B13" t="s">
-        <v>88</v>
+        <v>116</v>
       </c>
       <c r="C13">
         <v>6</v>
@@ -2404,12 +2949,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="A14" s="1">
         <v>2</v>
       </c>
       <c r="B14" t="s">
-        <v>88</v>
+        <v>116</v>
       </c>
       <c r="C14">
         <v>7</v>
@@ -2418,12 +2963,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4">
       <c r="A15" s="1">
         <v>2</v>
       </c>
       <c r="B15" t="s">
-        <v>88</v>
+        <v>116</v>
       </c>
       <c r="C15">
         <v>8</v>
@@ -2432,12 +2977,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4">
       <c r="A16" s="1">
         <v>2</v>
       </c>
       <c r="B16" t="s">
-        <v>88</v>
+        <v>116</v>
       </c>
       <c r="C16">
         <v>9</v>
@@ -2446,653 +2991,840 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3">
       <c r="A17" s="1">
         <v>3</v>
       </c>
       <c r="B17" t="s">
-        <v>89</v>
+        <v>117</v>
       </c>
       <c r="C17">
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3">
       <c r="A18" s="1">
         <v>3</v>
       </c>
       <c r="B18" t="s">
-        <v>89</v>
+        <v>117</v>
       </c>
       <c r="C18">
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3">
       <c r="A19" s="1">
         <v>3</v>
       </c>
       <c r="B19" t="s">
-        <v>89</v>
+        <v>117</v>
       </c>
       <c r="C19">
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3">
       <c r="A20" s="1">
         <v>4</v>
       </c>
       <c r="B20" t="s">
-        <v>89</v>
+        <v>117</v>
       </c>
       <c r="C20">
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3">
       <c r="A21" s="1">
         <v>4</v>
       </c>
       <c r="B21" t="s">
-        <v>90</v>
+        <v>118</v>
       </c>
       <c r="C21">
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3">
       <c r="A22" s="1">
         <v>4</v>
       </c>
       <c r="B22" t="s">
-        <v>89</v>
+        <v>117</v>
       </c>
       <c r="C22">
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3">
       <c r="A23" s="1">
         <v>4</v>
       </c>
       <c r="B23" t="s">
-        <v>89</v>
+        <v>117</v>
       </c>
       <c r="C23">
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3">
       <c r="A24" s="1">
         <v>4</v>
       </c>
       <c r="B24" t="s">
-        <v>89</v>
+        <v>117</v>
       </c>
       <c r="C24">
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3">
       <c r="A25" s="1">
         <v>4</v>
       </c>
       <c r="B25" t="s">
-        <v>89</v>
+        <v>117</v>
       </c>
       <c r="C25">
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3">
       <c r="A26" s="1">
         <v>5</v>
       </c>
       <c r="B26" t="s">
-        <v>89</v>
+        <v>117</v>
       </c>
       <c r="C26">
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3">
       <c r="A27" s="1">
         <v>5</v>
       </c>
       <c r="B27" t="s">
-        <v>89</v>
+        <v>117</v>
       </c>
       <c r="C27">
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3">
       <c r="A28" s="1">
         <v>5</v>
       </c>
       <c r="B28" t="s">
-        <v>89</v>
+        <v>117</v>
       </c>
       <c r="C28">
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3">
       <c r="A29" s="1">
         <v>6</v>
       </c>
       <c r="B29" t="s">
-        <v>89</v>
+        <v>117</v>
       </c>
       <c r="C29">
         <v>11</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3">
       <c r="A30" s="1">
         <v>6</v>
       </c>
       <c r="B30" t="s">
-        <v>89</v>
+        <v>117</v>
       </c>
       <c r="C30">
         <v>12</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3">
       <c r="A31" s="1">
         <v>6</v>
       </c>
       <c r="B31" t="s">
-        <v>89</v>
+        <v>117</v>
       </c>
       <c r="C31">
         <v>13</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3">
       <c r="A32" s="1">
         <v>7</v>
       </c>
       <c r="B32" t="s">
-        <v>89</v>
+        <v>117</v>
       </c>
       <c r="C32">
         <v>14</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3">
       <c r="A33" s="1">
         <v>7</v>
       </c>
       <c r="B33" t="s">
-        <v>89</v>
+        <v>117</v>
       </c>
       <c r="C33">
         <v>15</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3">
       <c r="A34" s="1">
         <v>8</v>
       </c>
       <c r="B34" t="s">
-        <v>89</v>
+        <v>117</v>
       </c>
       <c r="C34">
         <v>16</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3">
       <c r="A35" s="1">
         <v>8</v>
       </c>
       <c r="B35" t="s">
-        <v>89</v>
+        <v>117</v>
       </c>
       <c r="C35">
         <v>17</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3">
       <c r="A36" s="1">
         <v>9</v>
       </c>
       <c r="B36" t="s">
-        <v>90</v>
+        <v>118</v>
       </c>
       <c r="C36">
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3">
       <c r="A37" s="1">
         <v>9</v>
       </c>
       <c r="B37" t="s">
-        <v>90</v>
+        <v>118</v>
       </c>
       <c r="C37">
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3">
       <c r="A38" s="1">
         <v>10</v>
       </c>
       <c r="B38" t="s">
-        <v>89</v>
+        <v>117</v>
       </c>
       <c r="C38">
         <v>18</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3">
       <c r="A39" s="1">
         <v>10</v>
       </c>
       <c r="B39" t="s">
-        <v>89</v>
+        <v>117</v>
       </c>
       <c r="C39">
         <v>19</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3">
       <c r="A40" s="1">
         <v>10</v>
       </c>
       <c r="B40" t="s">
-        <v>89</v>
+        <v>117</v>
       </c>
       <c r="C40">
         <v>20</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3">
       <c r="A41" s="1">
         <v>11</v>
       </c>
       <c r="B41" t="s">
-        <v>89</v>
+        <v>117</v>
       </c>
       <c r="C41">
         <v>21</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3">
       <c r="A42" s="1">
         <v>11</v>
       </c>
       <c r="B42" t="s">
-        <v>89</v>
+        <v>117</v>
       </c>
       <c r="C42">
         <v>22</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3">
       <c r="A43" s="1">
         <v>12</v>
       </c>
       <c r="B43" t="s">
-        <v>90</v>
+        <v>118</v>
       </c>
       <c r="C43">
         <v>7</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3">
       <c r="A44" s="1">
         <v>12</v>
       </c>
       <c r="B44" t="s">
-        <v>90</v>
+        <v>118</v>
       </c>
       <c r="C44">
         <v>8</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3">
       <c r="A45" s="1">
         <v>13</v>
       </c>
       <c r="B45" t="s">
-        <v>89</v>
+        <v>117</v>
       </c>
       <c r="C45">
         <v>23</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3">
       <c r="A46" s="1">
         <v>13</v>
       </c>
       <c r="B46" t="s">
-        <v>89</v>
+        <v>117</v>
       </c>
       <c r="C46">
         <v>24</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3">
       <c r="A47" s="1">
         <v>14</v>
       </c>
       <c r="B47" t="s">
-        <v>89</v>
+        <v>117</v>
       </c>
       <c r="C47">
         <v>25</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3">
       <c r="A48" s="1">
         <v>14</v>
       </c>
       <c r="B48" t="s">
-        <v>90</v>
+        <v>118</v>
       </c>
       <c r="C48">
         <v>10</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3">
       <c r="A49" s="1">
         <v>15</v>
       </c>
       <c r="B49" t="s">
-        <v>90</v>
+        <v>118</v>
       </c>
       <c r="C49">
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3">
       <c r="A50" s="1">
         <v>15</v>
       </c>
       <c r="B50" t="s">
-        <v>90</v>
+        <v>118</v>
       </c>
       <c r="C50">
         <v>2</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3">
       <c r="A51" s="1">
         <v>15</v>
       </c>
       <c r="B51" t="s">
-        <v>90</v>
+        <v>118</v>
       </c>
       <c r="C51">
         <v>3</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3">
       <c r="A52" s="1">
         <v>15</v>
       </c>
       <c r="B52" t="s">
-        <v>90</v>
+        <v>118</v>
       </c>
       <c r="C52">
         <v>6</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3">
       <c r="A53" s="1">
         <v>15</v>
       </c>
       <c r="B53" t="s">
-        <v>90</v>
+        <v>118</v>
       </c>
       <c r="C53">
         <v>9</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3">
       <c r="A54" s="1">
         <v>15</v>
       </c>
       <c r="B54" t="s">
-        <v>90</v>
+        <v>118</v>
       </c>
       <c r="C54">
         <v>11</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3">
       <c r="A55" s="1">
         <v>16</v>
       </c>
       <c r="B55" t="s">
-        <v>89</v>
+        <v>117</v>
       </c>
       <c r="C55">
         <v>25</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3">
       <c r="A56" s="1">
         <v>16</v>
       </c>
       <c r="B56" t="s">
-        <v>89</v>
+        <v>117</v>
       </c>
       <c r="C56">
         <v>26</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3">
       <c r="A57" s="1">
         <v>16</v>
       </c>
       <c r="B57" t="s">
-        <v>89</v>
+        <v>117</v>
       </c>
       <c r="C57">
         <v>27</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3">
       <c r="A58" s="1">
         <v>16</v>
       </c>
       <c r="B58" t="s">
-        <v>89</v>
+        <v>117</v>
       </c>
       <c r="C58">
         <v>28</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3">
       <c r="A59" s="1">
         <v>16</v>
       </c>
       <c r="B59" t="s">
-        <v>89</v>
+        <v>117</v>
       </c>
       <c r="C59">
         <v>29</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3">
       <c r="A60" s="1">
         <v>16</v>
       </c>
       <c r="B60" t="s">
-        <v>89</v>
+        <v>117</v>
       </c>
       <c r="C60">
         <v>30</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3">
       <c r="A61" s="1">
         <v>16</v>
       </c>
       <c r="B61" t="s">
-        <v>89</v>
+        <v>117</v>
       </c>
       <c r="C61">
         <v>31</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3">
       <c r="A62" s="1">
         <v>16</v>
       </c>
       <c r="B62" t="s">
-        <v>89</v>
+        <v>117</v>
       </c>
       <c r="C62">
         <v>32</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3">
       <c r="A63" s="1">
         <v>16</v>
       </c>
       <c r="B63" t="s">
-        <v>89</v>
+        <v>117</v>
       </c>
       <c r="C63">
         <v>33</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3">
       <c r="A64" s="1">
         <v>17</v>
       </c>
       <c r="B64" t="s">
-        <v>89</v>
+        <v>117</v>
       </c>
       <c r="C64">
         <v>34</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3">
       <c r="A65" s="1">
         <v>17</v>
       </c>
       <c r="B65" t="s">
-        <v>89</v>
+        <v>117</v>
       </c>
       <c r="C65">
         <v>35</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3">
       <c r="A66" s="1">
         <v>17</v>
       </c>
       <c r="B66" t="s">
-        <v>89</v>
+        <v>117</v>
       </c>
       <c r="C66">
         <v>36</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3">
       <c r="A67" s="1">
         <v>17</v>
       </c>
       <c r="B67" t="s">
-        <v>89</v>
+        <v>117</v>
       </c>
       <c r="C67">
         <v>37</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3">
       <c r="A68" s="1">
         <v>17</v>
       </c>
       <c r="B68" t="s">
-        <v>89</v>
+        <v>117</v>
       </c>
       <c r="C68">
         <v>38</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3">
       <c r="A69" s="1">
         <v>17</v>
       </c>
       <c r="B69" t="s">
-        <v>89</v>
+        <v>117</v>
       </c>
       <c r="C69">
         <v>39</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3">
       <c r="A70" s="1">
         <v>17</v>
       </c>
       <c r="B70" t="s">
-        <v>89</v>
+        <v>117</v>
       </c>
       <c r="C70">
         <v>40</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3">
       <c r="A71" s="1">
         <v>17</v>
       </c>
       <c r="B71" t="s">
-        <v>89</v>
+        <v>117</v>
       </c>
       <c r="C71">
         <v>41</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3">
       <c r="A72" s="1">
         <v>17</v>
       </c>
       <c r="B72" t="s">
-        <v>89</v>
+        <v>117</v>
       </c>
       <c r="C72">
         <v>42</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3">
       <c r="A73" s="1">
         <v>17</v>
       </c>
       <c r="B73" t="s">
-        <v>89</v>
+        <v>117</v>
       </c>
       <c r="C73">
         <v>43</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3">
       <c r="A74" s="1">
         <v>17</v>
       </c>
       <c r="B74" t="s">
-        <v>89</v>
+        <v>117</v>
       </c>
       <c r="C74">
         <v>44</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:3">
       <c r="A75" s="1">
         <v>17</v>
       </c>
       <c r="B75" t="s">
-        <v>89</v>
+        <v>117</v>
       </c>
       <c r="C75">
         <v>45</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3">
+      <c r="A76" s="1">
+        <v>18</v>
+      </c>
+      <c r="B76" t="s">
+        <v>117</v>
+      </c>
+      <c r="C76">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3">
+      <c r="A77" s="1">
+        <v>18</v>
+      </c>
+      <c r="B77" t="s">
+        <v>117</v>
+      </c>
+      <c r="C77">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3">
+      <c r="A78" s="1">
+        <v>18</v>
+      </c>
+      <c r="B78" t="s">
+        <v>117</v>
+      </c>
+      <c r="C78">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3">
+      <c r="A79" s="1">
+        <v>19</v>
+      </c>
+      <c r="B79" t="s">
+        <v>117</v>
+      </c>
+      <c r="C79">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3">
+      <c r="A80" s="1">
+        <v>19</v>
+      </c>
+      <c r="B80" t="s">
+        <v>117</v>
+      </c>
+      <c r="C80">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3">
+      <c r="A81" s="1">
+        <v>19</v>
+      </c>
+      <c r="B81" t="s">
+        <v>117</v>
+      </c>
+      <c r="C81">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3">
+      <c r="A82" s="1">
+        <v>19</v>
+      </c>
+      <c r="B82" t="s">
+        <v>117</v>
+      </c>
+      <c r="C82">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3">
+      <c r="A83" s="1">
+        <v>19</v>
+      </c>
+      <c r="B83" t="s">
+        <v>117</v>
+      </c>
+      <c r="C83">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3">
+      <c r="A84" s="1">
+        <v>19</v>
+      </c>
+      <c r="B84" t="s">
+        <v>117</v>
+      </c>
+      <c r="C84">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3">
+      <c r="A85" s="1">
+        <v>19</v>
+      </c>
+      <c r="B85" t="s">
+        <v>117</v>
+      </c>
+      <c r="C85">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3">
+      <c r="A86" s="1">
+        <v>20</v>
+      </c>
+      <c r="B86" t="s">
+        <v>117</v>
+      </c>
+      <c r="C86">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3">
+      <c r="A87" s="1">
+        <v>20</v>
+      </c>
+      <c r="B87" t="s">
+        <v>117</v>
+      </c>
+      <c r="C87">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3">
+      <c r="A88" s="1">
+        <v>20</v>
+      </c>
+      <c r="B88" t="s">
+        <v>117</v>
+      </c>
+      <c r="C88">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3">
+      <c r="A89" s="1">
+        <v>21</v>
+      </c>
+      <c r="B89" t="s">
+        <v>117</v>
+      </c>
+      <c r="C89">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3">
+      <c r="A90" s="1">
+        <v>21</v>
+      </c>
+      <c r="B90" t="s">
+        <v>117</v>
+      </c>
+      <c r="C90">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3">
+      <c r="A91" s="1">
+        <v>21</v>
+      </c>
+      <c r="B91" t="s">
+        <v>117</v>
+      </c>
+      <c r="C91">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3">
+      <c r="A92" s="1">
+        <v>21</v>
+      </c>
+      <c r="B92" t="s">
+        <v>117</v>
+      </c>
+      <c r="C92">
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -3101,25 +3833,25 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>93</v>
+        <v>121</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>91</v>
+        <v>119</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -3127,10 +3859,10 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -3138,10 +3870,10 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -3149,10 +3881,10 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -3160,10 +3892,10 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -3171,10 +3903,10 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -3182,10 +3914,10 @@
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -3193,10 +3925,10 @@
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -3204,10 +3936,10 @@
         <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -3215,10 +3947,10 @@
         <v>3</v>
       </c>
       <c r="C10" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -3226,10 +3958,10 @@
         <v>4</v>
       </c>
       <c r="C11" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -3237,10 +3969,10 @@
         <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -3248,10 +3980,10 @@
         <v>2</v>
       </c>
       <c r="C13" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -3259,10 +3991,10 @@
         <v>3</v>
       </c>
       <c r="C14" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -3270,10 +4002,10 @@
         <v>4</v>
       </c>
       <c r="C15" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -3281,7 +4013,7 @@
         <v>5</v>
       </c>
       <c r="C16" t="s">
-        <v>108</v>
+        <v>136</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added more complex data models
</commit_message>
<xml_diff>
--- a/config/data_definitions.xlsx
+++ b/config/data_definitions.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18326"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\genkinjz\icu_ml_project\v5\config\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
@@ -12,7 +17,7 @@
     <sheet name="lists" sheetId="3" r:id="rId3"/>
     <sheet name="categories" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -211,9 +216,6 @@
     <t>central venous oxygen saturation</t>
   </si>
   <si>
-    <t>end tidal cardon dioxide</t>
-  </si>
-  <si>
     <t>beats/min</t>
   </si>
   <si>
@@ -428,13 +430,16 @@
   </si>
   <si>
     <t>Oriented</t>
+  </si>
+  <si>
+    <t>end tidal carbon dioxide</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -497,6 +502,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -543,7 +556,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -575,9 +588,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -609,6 +640,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -784,14 +833,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H75"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="B60" sqref="B60"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -817,7 +868,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -825,13 +876,13 @@
         <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F2">
         <v>0</v>
@@ -840,7 +891,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -848,13 +899,13 @@
         <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -863,7 +914,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -871,13 +922,13 @@
         <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F4">
         <v>0</v>
@@ -886,7 +937,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -894,13 +945,13 @@
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F5">
         <v>0</v>
@@ -909,7 +960,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -917,13 +968,13 @@
         <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F6">
         <v>0</v>
@@ -932,7 +983,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -940,13 +991,13 @@
         <v>13</v>
       </c>
       <c r="C7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F7">
         <v>0</v>
@@ -955,7 +1006,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -963,13 +1014,13 @@
         <v>14</v>
       </c>
       <c r="C8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F8">
         <v>0</v>
@@ -978,7 +1029,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -986,13 +1037,13 @@
         <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F9">
         <v>0</v>
@@ -1001,7 +1052,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -1009,13 +1060,13 @@
         <v>16</v>
       </c>
       <c r="C10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F10">
         <v>0</v>
@@ -1024,7 +1075,7 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -1032,13 +1083,13 @@
         <v>16</v>
       </c>
       <c r="C11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D11" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E11" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F11">
         <v>0</v>
@@ -1047,7 +1098,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -1055,13 +1106,13 @@
         <v>16</v>
       </c>
       <c r="C12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D12" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E12" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F12">
         <v>0</v>
@@ -1070,7 +1121,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -1078,19 +1129,19 @@
         <v>17</v>
       </c>
       <c r="C13" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E13" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H13">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -1098,19 +1149,19 @@
         <v>18</v>
       </c>
       <c r="C14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D14" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E14" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H14">
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -1118,19 +1169,19 @@
         <v>19</v>
       </c>
       <c r="C15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D15" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E15" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H15">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -1138,13 +1189,13 @@
         <v>20</v>
       </c>
       <c r="C16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D16" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E16" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F16">
         <v>0</v>
@@ -1153,7 +1204,7 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -1161,13 +1212,13 @@
         <v>20</v>
       </c>
       <c r="C17" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D17" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E17" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F17">
         <v>0</v>
@@ -1176,7 +1227,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -1184,13 +1235,13 @@
         <v>21</v>
       </c>
       <c r="C18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D18" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F18">
         <v>0</v>
@@ -1199,7 +1250,7 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -1207,13 +1258,13 @@
         <v>21</v>
       </c>
       <c r="C19" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D19" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E19" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F19">
         <v>0</v>
@@ -1222,7 +1273,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -1230,13 +1281,13 @@
         <v>22</v>
       </c>
       <c r="C20" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D20" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E20" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F20">
         <v>0</v>
@@ -1245,7 +1296,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -1253,13 +1304,13 @@
         <v>22</v>
       </c>
       <c r="C21" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D21" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E21" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F21">
         <v>0</v>
@@ -1268,7 +1319,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -1276,13 +1327,13 @@
         <v>22</v>
       </c>
       <c r="C22" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D22" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E22" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F22">
         <v>0</v>
@@ -1291,7 +1342,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -1302,10 +1353,10 @@
         <v>1</v>
       </c>
       <c r="D23" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E23" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F23">
         <v>0</v>
@@ -1314,7 +1365,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -1322,13 +1373,13 @@
         <v>23</v>
       </c>
       <c r="C24" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D24" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E24" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F24">
         <v>0</v>
@@ -1337,7 +1388,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -1345,13 +1396,13 @@
         <v>24</v>
       </c>
       <c r="C25" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D25" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E25" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F25">
         <v>0</v>
@@ -1360,7 +1411,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -1368,13 +1419,13 @@
         <v>24</v>
       </c>
       <c r="C26" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D26" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E26" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F26">
         <v>0</v>
@@ -1383,7 +1434,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -1391,13 +1442,13 @@
         <v>25</v>
       </c>
       <c r="C27" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D27" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E27" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F27">
         <v>0</v>
@@ -1406,7 +1457,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -1414,13 +1465,13 @@
         <v>26</v>
       </c>
       <c r="C28" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D28" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E28" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F28">
         <v>0</v>
@@ -1429,7 +1480,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -1437,13 +1488,13 @@
         <v>27</v>
       </c>
       <c r="C29" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D29" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E29" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F29">
         <v>0</v>
@@ -1452,7 +1503,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -1460,13 +1511,13 @@
         <v>28</v>
       </c>
       <c r="C30" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D30" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E30" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F30">
         <v>0</v>
@@ -1475,7 +1526,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -1483,13 +1534,13 @@
         <v>29</v>
       </c>
       <c r="C31" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D31" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E31" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F31">
         <v>0</v>
@@ -1498,7 +1549,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -1506,13 +1557,13 @@
         <v>30</v>
       </c>
       <c r="C32" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D32" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E32" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F32">
         <v>0</v>
@@ -1521,7 +1572,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -1529,13 +1580,13 @@
         <v>31</v>
       </c>
       <c r="C33" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D33" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E33" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F33">
         <v>0</v>
@@ -1544,7 +1595,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -1552,13 +1603,13 @@
         <v>32</v>
       </c>
       <c r="C34" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D34" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E34" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F34">
         <v>0</v>
@@ -1567,7 +1618,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="35" spans="1:7">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -1575,13 +1626,13 @@
         <v>33</v>
       </c>
       <c r="C35" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D35" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E35" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F35">
         <v>0</v>
@@ -1590,7 +1641,7 @@
         <v>5000000</v>
       </c>
     </row>
-    <row r="36" spans="1:7">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>34</v>
       </c>
@@ -1598,13 +1649,13 @@
         <v>34</v>
       </c>
       <c r="C36" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D36" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E36" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F36">
         <v>0</v>
@@ -1613,7 +1664,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="37" spans="1:7">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>35</v>
       </c>
@@ -1621,13 +1672,13 @@
         <v>34</v>
       </c>
       <c r="C37" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D37" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E37" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F37">
         <v>0</v>
@@ -1636,7 +1687,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="38" spans="1:7">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>36</v>
       </c>
@@ -1644,13 +1695,13 @@
         <v>35</v>
       </c>
       <c r="C38" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D38" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E38" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F38">
         <v>0</v>
@@ -1659,7 +1710,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="39" spans="1:7">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>37</v>
       </c>
@@ -1667,13 +1718,13 @@
         <v>35</v>
       </c>
       <c r="C39" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D39" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E39" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F39">
         <v>0</v>
@@ -1682,7 +1733,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="40" spans="1:7">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>38</v>
       </c>
@@ -1690,13 +1741,13 @@
         <v>36</v>
       </c>
       <c r="C40" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D40" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E40" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F40">
         <v>0</v>
@@ -1705,7 +1756,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="41" spans="1:7">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>39</v>
       </c>
@@ -1713,13 +1764,13 @@
         <v>37</v>
       </c>
       <c r="C41" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D41" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E41" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F41">
         <v>0</v>
@@ -1728,7 +1779,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="42" spans="1:7">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>40</v>
       </c>
@@ -1736,13 +1787,13 @@
         <v>38</v>
       </c>
       <c r="C42" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D42" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E42" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F42">
         <v>0</v>
@@ -1751,7 +1802,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="43" spans="1:7">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>41</v>
       </c>
@@ -1759,13 +1810,13 @@
         <v>38</v>
       </c>
       <c r="C43" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D43" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E43" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F43">
         <v>0</v>
@@ -1774,7 +1825,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="44" spans="1:7">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>42</v>
       </c>
@@ -1782,13 +1833,13 @@
         <v>39</v>
       </c>
       <c r="C44" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D44" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E44" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F44">
         <v>0</v>
@@ -1797,7 +1848,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="45" spans="1:7">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>43</v>
       </c>
@@ -1805,13 +1856,13 @@
         <v>39</v>
       </c>
       <c r="C45" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D45" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E45" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F45">
         <v>0</v>
@@ -1820,7 +1871,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="46" spans="1:7">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>44</v>
       </c>
@@ -1828,13 +1879,13 @@
         <v>40</v>
       </c>
       <c r="C46" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D46" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E46" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F46">
         <v>0</v>
@@ -1843,7 +1894,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="47" spans="1:7">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>45</v>
       </c>
@@ -1851,13 +1902,13 @@
         <v>40</v>
       </c>
       <c r="C47" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D47" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E47" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F47">
         <v>0</v>
@@ -1866,7 +1917,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="48" spans="1:7">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>46</v>
       </c>
@@ -1874,13 +1925,13 @@
         <v>41</v>
       </c>
       <c r="C48" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D48" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E48" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F48">
         <v>0</v>
@@ -1889,7 +1940,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="49" spans="1:7">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>47</v>
       </c>
@@ -1897,13 +1948,13 @@
         <v>41</v>
       </c>
       <c r="C49" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D49" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E49" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F49">
         <v>0</v>
@@ -1912,7 +1963,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="50" spans="1:7">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>48</v>
       </c>
@@ -1920,13 +1971,13 @@
         <v>42</v>
       </c>
       <c r="C50" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D50" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E50" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F50">
         <v>0</v>
@@ -1935,7 +1986,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="51" spans="1:7">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>49</v>
       </c>
@@ -1943,13 +1994,13 @@
         <v>42</v>
       </c>
       <c r="C51" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D51" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E51" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F51">
         <v>0</v>
@@ -1958,7 +2009,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="52" spans="1:7">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>50</v>
       </c>
@@ -1966,13 +2017,13 @@
         <v>43</v>
       </c>
       <c r="C52" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D52" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E52" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F52">
         <v>0</v>
@@ -1981,7 +2032,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="53" spans="1:7">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>51</v>
       </c>
@@ -1989,13 +2040,13 @@
         <v>43</v>
       </c>
       <c r="C53" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D53" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E53" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F53">
         <v>0</v>
@@ -2004,7 +2055,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="54" spans="1:7">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>52</v>
       </c>
@@ -2012,13 +2063,13 @@
         <v>44</v>
       </c>
       <c r="C54" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D54" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E54" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F54">
         <v>0</v>
@@ -2027,7 +2078,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="55" spans="1:7">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>53</v>
       </c>
@@ -2035,13 +2086,13 @@
         <v>45</v>
       </c>
       <c r="C55" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D55" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E55" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F55">
         <v>0</v>
@@ -2050,7 +2101,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="56" spans="1:7">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>54</v>
       </c>
@@ -2058,13 +2109,13 @@
         <v>46</v>
       </c>
       <c r="C56" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D56" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E56" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F56">
         <v>0</v>
@@ -2073,7 +2124,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="57" spans="1:7">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>55</v>
       </c>
@@ -2081,13 +2132,13 @@
         <v>47</v>
       </c>
       <c r="C57" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D57" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E57" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F57">
         <v>0</v>
@@ -2096,7 +2147,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="58" spans="1:7">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>56</v>
       </c>
@@ -2104,13 +2155,13 @@
         <v>48</v>
       </c>
       <c r="C58" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D58" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E58" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F58">
         <v>0</v>
@@ -2119,7 +2170,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="59" spans="1:7">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>57</v>
       </c>
@@ -2127,13 +2178,13 @@
         <v>49</v>
       </c>
       <c r="C59" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D59" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E59" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F59">
         <v>0</v>
@@ -2142,7 +2193,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="60" spans="1:7">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>58</v>
       </c>
@@ -2150,13 +2201,13 @@
         <v>50</v>
       </c>
       <c r="C60" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D60" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E60" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F60">
         <v>0</v>
@@ -2165,7 +2216,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="61" spans="1:7">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>59</v>
       </c>
@@ -2173,13 +2224,13 @@
         <v>51</v>
       </c>
       <c r="C61" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D61" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E61" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F61">
         <v>0</v>
@@ -2188,7 +2239,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="62" spans="1:7">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>60</v>
       </c>
@@ -2196,13 +2247,13 @@
         <v>52</v>
       </c>
       <c r="C62" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D62" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E62" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F62">
         <v>0</v>
@@ -2211,7 +2262,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="63" spans="1:7">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>61</v>
       </c>
@@ -2219,13 +2270,13 @@
         <v>53</v>
       </c>
       <c r="C63" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D63" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E63" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F63">
         <v>0</v>
@@ -2234,7 +2285,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="64" spans="1:7">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>62</v>
       </c>
@@ -2242,13 +2293,13 @@
         <v>54</v>
       </c>
       <c r="C64" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D64" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E64" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F64">
         <v>0</v>
@@ -2257,7 +2308,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="65" spans="1:7">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>63</v>
       </c>
@@ -2265,13 +2316,13 @@
         <v>55</v>
       </c>
       <c r="C65" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D65" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E65" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F65">
         <v>0</v>
@@ -2280,7 +2331,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="66" spans="1:7">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>64</v>
       </c>
@@ -2288,13 +2339,13 @@
         <v>56</v>
       </c>
       <c r="C66" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D66" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E66" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F66">
         <v>0</v>
@@ -2303,7 +2354,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="67" spans="1:7">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>65</v>
       </c>
@@ -2311,13 +2362,13 @@
         <v>57</v>
       </c>
       <c r="C67" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D67" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E67" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F67">
         <v>0</v>
@@ -2326,7 +2377,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="68" spans="1:7">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>66</v>
       </c>
@@ -2334,13 +2385,13 @@
         <v>58</v>
       </c>
       <c r="C68" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D68" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E68" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F68">
         <v>0</v>
@@ -2349,7 +2400,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="69" spans="1:7">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>67</v>
       </c>
@@ -2357,13 +2408,13 @@
         <v>59</v>
       </c>
       <c r="C69" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D69" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E69" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F69">
         <v>0</v>
@@ -2372,7 +2423,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="70" spans="1:7">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>68</v>
       </c>
@@ -2380,13 +2431,13 @@
         <v>59</v>
       </c>
       <c r="C70" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D70" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E70" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F70">
         <v>0</v>
@@ -2395,7 +2446,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:7">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>69</v>
       </c>
@@ -2403,13 +2454,13 @@
         <v>60</v>
       </c>
       <c r="C71" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D71" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E71" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F71">
         <v>0</v>
@@ -2418,7 +2469,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="72" spans="1:7">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>70</v>
       </c>
@@ -2426,13 +2477,13 @@
         <v>61</v>
       </c>
       <c r="C72" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D72" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E72" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F72">
         <v>0</v>
@@ -2441,7 +2492,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="73" spans="1:7">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>71</v>
       </c>
@@ -2449,13 +2500,13 @@
         <v>62</v>
       </c>
       <c r="C73" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D73" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E73" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F73">
         <v>0</v>
@@ -2464,7 +2515,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="74" spans="1:7">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>72</v>
       </c>
@@ -2472,13 +2523,13 @@
         <v>63</v>
       </c>
       <c r="C74" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D74" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E74" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F74">
         <v>0</v>
@@ -2487,21 +2538,21 @@
         <v>100</v>
       </c>
     </row>
-    <row r="75" spans="1:7">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>73</v>
       </c>
       <c r="B75" t="s">
-        <v>64</v>
+        <v>136</v>
       </c>
       <c r="C75" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D75" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E75" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F75">
         <v>0</v>
@@ -2516,69 +2567,69 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C2">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C3">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C4">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C5">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -2589,7 +2640,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -2600,18 +2651,18 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C8">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -2622,7 +2673,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -2633,18 +2684,18 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C11">
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -2655,100 +2706,100 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C13">
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C14">
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C15">
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C16">
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C17">
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C18">
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C19">
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C20">
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C21">
         <v>21</v>
@@ -2760,34 +2811,34 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D92"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="D1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="1">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>116</v>
-      </c>
       <c r="C2">
         <v>0</v>
       </c>
@@ -2795,12 +2846,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -2809,12 +2860,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>0</v>
       </c>
       <c r="B4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C4">
         <v>2</v>
@@ -2823,12 +2874,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>0</v>
       </c>
       <c r="B5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C5">
         <v>3</v>
@@ -2837,12 +2888,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>0</v>
       </c>
       <c r="B6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C6">
         <v>4</v>
@@ -2851,12 +2902,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>0</v>
       </c>
       <c r="B7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C7">
         <v>5</v>
@@ -2865,12 +2916,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C8">
         <v>10</v>
@@ -2879,12 +2930,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C9">
         <v>11</v>
@@ -2893,12 +2944,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C10">
         <v>12</v>
@@ -2907,12 +2958,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C11">
         <v>13</v>
@@ -2921,12 +2972,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>1</v>
       </c>
       <c r="B12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C12">
         <v>14</v>
@@ -2935,12 +2986,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>2</v>
       </c>
       <c r="B13" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C13">
         <v>6</v>
@@ -2949,12 +3000,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>2</v>
       </c>
       <c r="B14" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C14">
         <v>7</v>
@@ -2963,12 +3014,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>2</v>
       </c>
       <c r="B15" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C15">
         <v>8</v>
@@ -2977,12 +3028,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>2</v>
       </c>
       <c r="B16" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C16">
         <v>9</v>
@@ -2991,837 +3042,837 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>3</v>
       </c>
       <c r="B17" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C17">
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>3</v>
       </c>
       <c r="B18" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C18">
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>3</v>
       </c>
       <c r="B19" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C19">
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>4</v>
       </c>
       <c r="B20" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C20">
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>4</v>
       </c>
       <c r="B21" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C21">
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>4</v>
       </c>
       <c r="B22" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C22">
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>4</v>
       </c>
       <c r="B23" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C23">
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>4</v>
       </c>
       <c r="B24" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C24">
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>4</v>
       </c>
       <c r="B25" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C25">
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>5</v>
       </c>
       <c r="B26" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C26">
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>5</v>
       </c>
       <c r="B27" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C27">
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>5</v>
       </c>
       <c r="B28" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C28">
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>6</v>
       </c>
       <c r="B29" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C29">
         <v>11</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>6</v>
       </c>
       <c r="B30" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C30">
         <v>12</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>6</v>
       </c>
       <c r="B31" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C31">
         <v>13</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>7</v>
       </c>
       <c r="B32" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C32">
         <v>14</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>7</v>
       </c>
       <c r="B33" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C33">
         <v>15</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>8</v>
       </c>
       <c r="B34" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C34">
         <v>16</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>8</v>
       </c>
       <c r="B35" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C35">
         <v>17</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>9</v>
       </c>
       <c r="B36" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C36">
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="1:3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>9</v>
       </c>
       <c r="B37" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C37">
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="1:3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>10</v>
       </c>
       <c r="B38" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C38">
         <v>18</v>
       </c>
     </row>
-    <row r="39" spans="1:3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>10</v>
       </c>
       <c r="B39" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C39">
         <v>19</v>
       </c>
     </row>
-    <row r="40" spans="1:3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>10</v>
       </c>
       <c r="B40" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C40">
         <v>20</v>
       </c>
     </row>
-    <row r="41" spans="1:3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>11</v>
       </c>
       <c r="B41" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C41">
         <v>21</v>
       </c>
     </row>
-    <row r="42" spans="1:3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>11</v>
       </c>
       <c r="B42" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C42">
         <v>22</v>
       </c>
     </row>
-    <row r="43" spans="1:3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>12</v>
       </c>
       <c r="B43" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C43">
         <v>7</v>
       </c>
     </row>
-    <row r="44" spans="1:3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>12</v>
       </c>
       <c r="B44" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C44">
         <v>8</v>
       </c>
     </row>
-    <row r="45" spans="1:3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>13</v>
       </c>
       <c r="B45" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C45">
         <v>23</v>
       </c>
     </row>
-    <row r="46" spans="1:3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>13</v>
       </c>
       <c r="B46" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C46">
         <v>24</v>
       </c>
     </row>
-    <row r="47" spans="1:3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>14</v>
       </c>
       <c r="B47" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C47">
         <v>25</v>
       </c>
     </row>
-    <row r="48" spans="1:3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>14</v>
       </c>
       <c r="B48" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C48">
         <v>10</v>
       </c>
     </row>
-    <row r="49" spans="1:3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>15</v>
       </c>
       <c r="B49" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C49">
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>15</v>
       </c>
       <c r="B50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C50">
         <v>2</v>
       </c>
     </row>
-    <row r="51" spans="1:3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>15</v>
       </c>
       <c r="B51" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C51">
         <v>3</v>
       </c>
     </row>
-    <row r="52" spans="1:3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>15</v>
       </c>
       <c r="B52" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C52">
         <v>6</v>
       </c>
     </row>
-    <row r="53" spans="1:3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>15</v>
       </c>
       <c r="B53" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C53">
         <v>9</v>
       </c>
     </row>
-    <row r="54" spans="1:3">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>15</v>
       </c>
       <c r="B54" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C54">
         <v>11</v>
       </c>
     </row>
-    <row r="55" spans="1:3">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>16</v>
       </c>
       <c r="B55" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C55">
         <v>25</v>
       </c>
     </row>
-    <row r="56" spans="1:3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>16</v>
       </c>
       <c r="B56" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C56">
         <v>26</v>
       </c>
     </row>
-    <row r="57" spans="1:3">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>16</v>
       </c>
       <c r="B57" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C57">
         <v>27</v>
       </c>
     </row>
-    <row r="58" spans="1:3">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>16</v>
       </c>
       <c r="B58" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C58">
         <v>28</v>
       </c>
     </row>
-    <row r="59" spans="1:3">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>16</v>
       </c>
       <c r="B59" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C59">
         <v>29</v>
       </c>
     </row>
-    <row r="60" spans="1:3">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>16</v>
       </c>
       <c r="B60" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C60">
         <v>30</v>
       </c>
     </row>
-    <row r="61" spans="1:3">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>16</v>
       </c>
       <c r="B61" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C61">
         <v>31</v>
       </c>
     </row>
-    <row r="62" spans="1:3">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>16</v>
       </c>
       <c r="B62" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C62">
         <v>32</v>
       </c>
     </row>
-    <row r="63" spans="1:3">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>16</v>
       </c>
       <c r="B63" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C63">
         <v>33</v>
       </c>
     </row>
-    <row r="64" spans="1:3">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>17</v>
       </c>
       <c r="B64" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C64">
         <v>34</v>
       </c>
     </row>
-    <row r="65" spans="1:3">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>17</v>
       </c>
       <c r="B65" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C65">
         <v>35</v>
       </c>
     </row>
-    <row r="66" spans="1:3">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>17</v>
       </c>
       <c r="B66" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C66">
         <v>36</v>
       </c>
     </row>
-    <row r="67" spans="1:3">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>17</v>
       </c>
       <c r="B67" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C67">
         <v>37</v>
       </c>
     </row>
-    <row r="68" spans="1:3">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>17</v>
       </c>
       <c r="B68" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C68">
         <v>38</v>
       </c>
     </row>
-    <row r="69" spans="1:3">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>17</v>
       </c>
       <c r="B69" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C69">
         <v>39</v>
       </c>
     </row>
-    <row r="70" spans="1:3">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>17</v>
       </c>
       <c r="B70" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C70">
         <v>40</v>
       </c>
     </row>
-    <row r="71" spans="1:3">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>17</v>
       </c>
       <c r="B71" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C71">
         <v>41</v>
       </c>
     </row>
-    <row r="72" spans="1:3">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>17</v>
       </c>
       <c r="B72" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C72">
         <v>42</v>
       </c>
     </row>
-    <row r="73" spans="1:3">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>17</v>
       </c>
       <c r="B73" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C73">
         <v>43</v>
       </c>
     </row>
-    <row r="74" spans="1:3">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>17</v>
       </c>
       <c r="B74" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C74">
         <v>44</v>
       </c>
     </row>
-    <row r="75" spans="1:3">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>17</v>
       </c>
       <c r="B75" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C75">
         <v>45</v>
       </c>
     </row>
-    <row r="76" spans="1:3">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>18</v>
       </c>
       <c r="B76" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C76">
         <v>54</v>
       </c>
     </row>
-    <row r="77" spans="1:3">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>18</v>
       </c>
       <c r="B77" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C77">
         <v>55</v>
       </c>
     </row>
-    <row r="78" spans="1:3">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>18</v>
       </c>
       <c r="B78" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C78">
         <v>56</v>
       </c>
     </row>
-    <row r="79" spans="1:3">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>19</v>
       </c>
       <c r="B79" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C79">
         <v>23</v>
       </c>
     </row>
-    <row r="80" spans="1:3">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>19</v>
       </c>
       <c r="B80" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C80">
         <v>24</v>
       </c>
     </row>
-    <row r="81" spans="1:3">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>19</v>
       </c>
       <c r="B81" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C81">
         <v>57</v>
       </c>
     </row>
-    <row r="82" spans="1:3">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>19</v>
       </c>
       <c r="B82" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C82">
         <v>58</v>
       </c>
     </row>
-    <row r="83" spans="1:3">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>19</v>
       </c>
       <c r="B83" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C83">
         <v>59</v>
       </c>
     </row>
-    <row r="84" spans="1:3">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>19</v>
       </c>
       <c r="B84" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C84">
         <v>60</v>
       </c>
     </row>
-    <row r="85" spans="1:3">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>19</v>
       </c>
       <c r="B85" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C85">
         <v>62</v>
       </c>
     </row>
-    <row r="86" spans="1:3">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>20</v>
       </c>
       <c r="B86" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C86">
         <v>64</v>
       </c>
     </row>
-    <row r="87" spans="1:3">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>20</v>
       </c>
       <c r="B87" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C87">
         <v>65</v>
       </c>
     </row>
-    <row r="88" spans="1:3">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>20</v>
       </c>
       <c r="B88" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C88">
         <v>66</v>
       </c>
     </row>
-    <row r="89" spans="1:3">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>21</v>
       </c>
       <c r="B89" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C89">
         <v>67</v>
       </c>
     </row>
-    <row r="90" spans="1:3">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>21</v>
       </c>
       <c r="B90" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C90">
         <v>68</v>
       </c>
     </row>
-    <row r="91" spans="1:3">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <v>21</v>
       </c>
       <c r="B91" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C91">
         <v>69</v>
       </c>
     </row>
-    <row r="92" spans="1:3">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <v>21</v>
       </c>
       <c r="B92" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C92">
         <v>70</v>
@@ -3833,25 +3884,25 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -3859,10 +3910,10 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -3870,10 +3921,10 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -3881,10 +3932,10 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -3892,10 +3943,10 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -3903,10 +3954,10 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -3914,10 +3965,10 @@
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -3925,10 +3976,10 @@
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -3936,10 +3987,10 @@
         <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -3947,10 +3998,10 @@
         <v>3</v>
       </c>
       <c r="C10" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -3958,10 +4009,10 @@
         <v>4</v>
       </c>
       <c r="C11" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -3969,10 +4020,10 @@
         <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -3980,10 +4031,10 @@
         <v>2</v>
       </c>
       <c r="C13" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -3991,10 +4042,10 @@
         <v>3</v>
       </c>
       <c r="C14" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -4002,10 +4053,10 @@
         <v>4</v>
       </c>
       <c r="C15" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -4013,7 +4064,7 @@
         <v>5</v>
       </c>
       <c r="C16" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
   </sheetData>

</xml_diff>